<commit_message>
updated stats about validation
</commit_message>
<xml_diff>
--- a/validation_data.xlsx
+++ b/validation_data.xlsx
@@ -524,10 +524,11 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -850,16 +851,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -875,6 +876,9 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
       <c r="G1" t="s">
         <v>4</v>
       </c>
@@ -897,6 +901,10 @@
         <f>ABS(A2-B2)</f>
         <v>1</v>
       </c>
+      <c r="E2" s="3">
+        <f>1 - (D2/A2)</f>
+        <v>0.96666666666666667</v>
+      </c>
       <c r="G2" t="s">
         <v>3</v>
       </c>
@@ -919,6 +927,10 @@
         <f t="shared" ref="D3:D18" si="0">ABS(A3-B3)</f>
         <v>1</v>
       </c>
+      <c r="E3" s="3">
+        <f t="shared" ref="E3:E18" si="1">1 - (D3/A3)</f>
+        <v>0.96551724137931039</v>
+      </c>
       <c r="G3" t="s">
         <v>5</v>
       </c>
@@ -941,6 +953,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="E4" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
       <c r="G4" t="s">
         <v>5</v>
       </c>
@@ -963,13 +979,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="2">
-        <f>1 - AVERAGE(ABS(A2:A18-B2:B18)/A2:A18)</f>
-        <v>1</v>
-      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -985,6 +999,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1000,6 +1018,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="E7" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95833333333333337</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1015,6 +1037,10 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
+      <c r="E8" s="3">
+        <f t="shared" si="1"/>
+        <v>0.93103448275862066</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1030,6 +1056,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="E9" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1045,6 +1075,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="E10" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1060,6 +1094,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="E11" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1075,6 +1113,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="E12" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1090,6 +1132,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="E13" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1105,6 +1151,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="E14" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1120,6 +1170,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="E15" s="3">
+        <f t="shared" si="1"/>
+        <v>0.98717948717948723</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -1135,8 +1189,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>39</v>
       </c>
@@ -1150,8 +1208,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>26</v>
       </c>
@@ -1165,9 +1227,98 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
+      <c r="E18" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <f t="shared" ref="A21:B21" si="2">AVERAGE(A2:A18)</f>
+        <v>35.647058823529413</v>
+      </c>
+      <c r="B21" s="1">
+        <f t="shared" si="2"/>
+        <v>35.764705882352942</v>
+      </c>
+      <c r="C21" s="1">
+        <f>AVERAGE(C2:C18)</f>
+        <v>23.529411764705884</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" ref="D21:E21" si="3">AVERAGE(D2:D18)</f>
+        <v>0.35294117647058826</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="3"/>
+        <v>0.98874889478337757</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <f t="shared" ref="A22:B22" si="4">STDEV(A2:A18)</f>
+        <v>14.339374012097718</v>
+      </c>
+      <c r="B22" s="1">
+        <f t="shared" si="4"/>
+        <v>14.493659871495131</v>
+      </c>
+      <c r="C22" s="1">
+        <f>STDEV(C2:C18)</f>
+        <v>8.1556548408054237</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" ref="D22:E22" si="5">STDEV(D2:D18)</f>
+        <v>0.60633906259083248</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="5"/>
+        <v>2.062296310478812E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f>MAX(A2:A18)</f>
+        <v>78</v>
+      </c>
+      <c r="B23">
+        <f t="shared" ref="B23:E23" si="6">MAX(B2:B18)</f>
+        <v>79</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="6"/>
+        <v>41</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f>MIN(A2:A18)</f>
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <f t="shared" ref="B24:E24" si="7">MIN(B2:B18)</f>
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="7"/>
+        <v>14</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="7"/>
+        <v>0.93103448275862066</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>